<commit_message>
shear wall work continue
</commit_message>
<xml_diff>
--- a/tools/bldg_layout.xlsx
+++ b/tools/bldg_layout.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hgp\Documents\bezerkeley\research\isol-sys-database\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D276E3-8993-4429-ADCF-1599BDF4F5C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850584C2-87EB-4D63-8526-3CA61DC430BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,10 +93,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,7 +379,7 @@
   <dimension ref="B3:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,11 +390,11 @@
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
@@ -406,7 +405,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>

</xml_diff>